<commit_message>
resimulated custom vs fanduel w/ $5 bets
</commit_message>
<xml_diff>
--- a/src/main/resources/analytics/FinalResultsOfStrategyVsRules.xlsx
+++ b/src/main/resources/analytics/FinalResultsOfStrategyVsRules.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Coding\BlackjackSimulator\src\main\resources\analytics\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arthurchan/IdeaProjects/BlackjackSimulator/src/main/resources/analytics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDC84EC4-AC20-4BB6-8322-014F87489F97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26094E20-4957-1F4A-96F3-2C7F25820007}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="17280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="15360" windowHeight="17280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -165,7 +165,7 @@
       <sheetData sheetId="0">
         <row r="11">
           <cell r="B11">
-            <v>5.3054817140445317E-3</v>
+            <v>3.4725109610900069E-3</v>
           </cell>
         </row>
       </sheetData>
@@ -453,12 +453,12 @@
       <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="3"/>
       <c r="B1" s="3"/>
       <c r="C1" s="3" t="s">
@@ -466,7 +466,7 @@
       </c>
       <c r="D1" s="3"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="2" t="s">
@@ -476,7 +476,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
@@ -486,7 +486,7 @@
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="4"/>
       <c r="B4" s="2" t="s">
         <v>5</v>
@@ -494,15 +494,15 @@
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="4"/>
       <c r="B5" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1">
-        <f ca="1">[1]Results!$B$11</f>
-        <v>5.3054817140445317E-3</v>
+        <f>[1]Results!$B$11</f>
+        <v>3.4725109610900069E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>